<commit_message>
add plans for sprint1 and models
</commit_message>
<xml_diff>
--- a/docs/Module list.xlsx
+++ b/docs/Module list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Small Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tech Blog\TechBlog-Client\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Module</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>the rule haven't been decided yet, we can use a large pic to hold the place</t>
+  </si>
+  <si>
+    <t>can give comment to the post or specific comment</t>
   </si>
 </sst>
 </file>
@@ -485,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,37 +639,43 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>